<commit_message>
Revisar EDA y 2/3 partes hechas del dashboard
</commit_message>
<xml_diff>
--- a/Datasets/data.xlsx
+++ b/Datasets/data.xlsx
@@ -475,12 +475,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>longitud</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>latitud</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>longitud</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">

</xml_diff>